<commit_message>
modify new file generation remove filter in ERRORS tab
</commit_message>
<xml_diff>
--- a/multiplexSimoaGenerator/src/main/java/com/multiplexSimoaGenerator/neuro4plex_Model.xlsx
+++ b/multiplexSimoaGenerator/src/main/java/com/multiplexSimoaGenerator/neuro4plex_Model.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\projects\multiplexSimoaGenerator\src\com\multiplexSimoaGenerator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{F410F809-1F32-4AAA-B566-ACBCDEAF602B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{4B36BB5D-7598-4892-88B3-F433F915C9C1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAB" sheetId="3" r:id="rId1"/>
@@ -20,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ERRORS!$A$1:$AN$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
+  <oleSize ref="A27:J46"/>
 </workbook>
 </file>
 
@@ -177,7 +173,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -718,7 +714,7 @@
     <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,8 +1101,8 @@
   </sheetPr>
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="97" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L49"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,8 +2467,8 @@
   </sheetPr>
   <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="97" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2605,11 +2601,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN1" xr:uid="{00000000-0009-0000-0000-000006000000}">
-    <sortState ref="A2:AN329">
-      <sortCondition ref="H1:H329"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tri + generation fichier ok
</commit_message>
<xml_diff>
--- a/multiplexSimoaGenerator/src/main/java/com/multiplexSimoaGenerator/neuro4plex_Model.xlsx
+++ b/multiplexSimoaGenerator/src/main/java/com/multiplexSimoaGenerator/neuro4plex_Model.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{4B36BB5D-7598-4892-88B3-F433F915C9C1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\git\mutiplexSimoaGenerator\multiplexSimoaGenerator\src\main\java\com\multiplexSimoaGenerator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6B210592-B9B3-4F41-B314-1070616E3BF7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,8 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ERRORS!$A$1:$AN$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
-  <oleSize ref="A27:J46"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -175,7 +179,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,15 +318,6 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <strike/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -634,21 +629,21 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -696,67 +691,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -803,7 +787,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1099,139 +1093,140 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.7109375" style="5" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="14" style="18" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="7"/>
-    <col min="8" max="8" width="9.140625" style="19"/>
-    <col min="9" max="9" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="18"/>
-    <col min="11" max="11" width="12.85546875" style="20" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="10" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="10"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="9.140625" style="18"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="12.85546875" style="19" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="e">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="e">
         <f t="shared" ref="H2:H9" si="0">AVERAGE(F2:G2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I2" s="9" t="e">
+      <c r="I2" s="14" t="e">
         <f t="shared" ref="I2:I9" si="1">_xlfn.STDEV.S(F2:G2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J2" s="10" t="e">
+      <c r="J2" s="15" t="e">
         <f t="shared" ref="J2:J9" si="2">100*I2/AVERAGE(F2:G2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="10">
+      <c r="K2" s="16"/>
+      <c r="L2" s="15">
         <f t="shared" ref="L2:L49" si="3">E2*10^K2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="e">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I3" s="9" t="e">
+      <c r="I3" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J3" s="10" t="e">
+      <c r="J3" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10">
+      <c r="K3" s="16"/>
+      <c r="L3" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8" t="e">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I4" s="9" t="e">
+      <c r="I4" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="10" t="e">
+      <c r="J4" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="10">
+      <c r="K4" s="16"/>
+      <c r="L4" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1239,27 +1234,27 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8" t="e">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="9" t="e">
+      <c r="I5" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="10" t="e">
+      <c r="J5" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="10">
+      <c r="K5" s="16"/>
+      <c r="L5" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1267,27 +1262,27 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8" t="e">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="9" t="e">
+      <c r="I6" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="10" t="e">
+      <c r="J6" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="10">
+      <c r="K6" s="16"/>
+      <c r="L6" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1295,27 +1290,27 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="8" t="e">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="9" t="e">
+      <c r="I7" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="10" t="e">
+      <c r="J7" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="10">
+      <c r="K7" s="16"/>
+      <c r="L7" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1323,27 +1318,27 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8" t="e">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="9" t="e">
+      <c r="I8" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="10" t="e">
+      <c r="J8" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="10">
+      <c r="K8" s="16"/>
+      <c r="L8" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1351,27 +1346,27 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8" t="e">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="9" t="e">
+      <c r="I9" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="10" t="e">
+      <c r="J9" s="15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="10">
+      <c r="K9" s="16"/>
+      <c r="L9" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1379,27 +1374,27 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="8" t="e">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="e">
         <f t="shared" ref="H10:H16" si="4">AVERAGE(F10:G10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="9" t="e">
+      <c r="I10" s="14" t="e">
         <f t="shared" ref="I10:I16" si="5">_xlfn.STDEV.S(F10:G10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="10" t="e">
+      <c r="J10" s="15" t="e">
         <f t="shared" ref="J10:J16" si="6">100*I10/AVERAGE(F10:G10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="16"/>
-      <c r="L10" s="10">
+      <c r="L10" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1407,27 +1402,27 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="8" t="e">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="9" t="e">
+      <c r="I11" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="10" t="e">
+      <c r="J11" s="15" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="10">
+      <c r="L11" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1435,27 +1430,27 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8" t="e">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I12" s="9" t="e">
+      <c r="I12" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="10" t="e">
+      <c r="J12" s="15" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="10">
+      <c r="K12" s="16"/>
+      <c r="L12" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1463,27 +1458,27 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8" t="e">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="9" t="e">
+      <c r="I13" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="10" t="e">
+      <c r="J13" s="15" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="10">
+      <c r="K13" s="16"/>
+      <c r="L13" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1491,53 +1486,53 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8" t="e">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I14" s="9" t="e">
+      <c r="I14" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="10" t="e">
+      <c r="J14" s="15" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="10">
+      <c r="K14" s="16"/>
+      <c r="L14" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8" t="e">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="9" t="e">
+      <c r="I15" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="10" t="e">
+      <c r="J15" s="15" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="10">
+      <c r="K15" s="16"/>
+      <c r="L15" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1545,79 +1540,79 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8" t="e">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I16" s="9" t="e">
+      <c r="I16" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" s="10" t="e">
+      <c r="J16" s="15" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="10">
+      <c r="K16" s="16"/>
+      <c r="L16" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8" t="e">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13" t="e">
         <f t="shared" ref="H17:H49" si="7">AVERAGE(F17:G17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I17" s="9" t="e">
+      <c r="I17" s="14" t="e">
         <f t="shared" ref="I17:I49" si="8">_xlfn.STDEV.S(F17:G17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J17" s="10" t="e">
+      <c r="J17" s="15" t="e">
         <f t="shared" ref="J17:J49" si="9">100*I17/AVERAGE(F17:G17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="10">
+      <c r="K17" s="16"/>
+      <c r="L17" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8" t="e">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I18" s="9" t="e">
+      <c r="I18" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" s="10" t="e">
+      <c r="J18" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="10">
+      <c r="K18" s="16"/>
+      <c r="L18" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1625,27 +1620,27 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8" t="e">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I19" s="9" t="e">
+      <c r="I19" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J19" s="10" t="e">
+      <c r="J19" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="10">
+      <c r="K19" s="16"/>
+      <c r="L19" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1654,27 +1649,27 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8" t="e">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I20" s="9" t="e">
+      <c r="I20" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="10" t="e">
+      <c r="J20" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K20" s="17"/>
-      <c r="L20" s="10">
+      <c r="K20" s="16"/>
+      <c r="L20" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1682,775 +1677,1892 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8" t="e">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" s="9" t="e">
+      <c r="I21" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J21" s="10" t="e">
+      <c r="J21" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="10">
+      <c r="K21" s="16"/>
+      <c r="L21" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="8" t="e">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I22" s="9" t="e">
+      <c r="I22" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J22" s="10" t="e">
+      <c r="J22" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="10">
+      <c r="K22" s="16"/>
+      <c r="L22" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="8" t="e">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I23" s="9" t="e">
+      <c r="I23" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J23" s="10" t="e">
+      <c r="J23" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="10">
+      <c r="K23" s="16"/>
+      <c r="L23" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="8" t="e">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I24" s="9" t="e">
+      <c r="I24" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J24" s="10" t="e">
+      <c r="J24" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="10">
+      <c r="K24" s="16"/>
+      <c r="L24" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="8" t="e">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I25" s="9" t="e">
+      <c r="I25" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J25" s="10" t="e">
+      <c r="J25" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="10">
+      <c r="K25" s="16"/>
+      <c r="L25" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="8" t="e">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I26" s="9" t="e">
+      <c r="I26" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J26" s="10" t="e">
+      <c r="J26" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="10">
+      <c r="K26" s="16"/>
+      <c r="L26" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="8" t="e">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I27" s="9" t="e">
+      <c r="I27" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J27" s="10" t="e">
+      <c r="J27" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="10">
+      <c r="K27" s="16"/>
+      <c r="L27" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="8" t="e">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="9" t="e">
+      <c r="I28" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J28" s="10" t="e">
+      <c r="J28" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="10">
+      <c r="K28" s="16"/>
+      <c r="L28" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="8" t="e">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="9" t="e">
+      <c r="I29" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J29" s="10" t="e">
+      <c r="J29" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="10">
+      <c r="K29" s="16"/>
+      <c r="L29" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="8" t="e">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I30" s="9" t="e">
+      <c r="I30" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J30" s="10" t="e">
+      <c r="J30" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="10">
+      <c r="K30" s="16"/>
+      <c r="L30" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="8" t="e">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I31" s="9" t="e">
+      <c r="I31" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J31" s="10" t="e">
+      <c r="J31" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K31" s="17"/>
-      <c r="L31" s="10">
+      <c r="K31" s="16"/>
+      <c r="L31" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="8" t="e">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="9" t="e">
+      <c r="I32" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J32" s="10" t="e">
+      <c r="J32" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K32" s="17"/>
-      <c r="L32" s="10">
+      <c r="K32" s="16"/>
+      <c r="L32" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="8" t="e">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="9" t="e">
+      <c r="I33" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J33" s="10" t="e">
+      <c r="J33" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="10">
+      <c r="K33" s="16"/>
+      <c r="L33" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="8" t="e">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I34" s="9" t="e">
+      <c r="I34" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J34" s="10" t="e">
+      <c r="J34" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K34" s="17"/>
-      <c r="L34" s="10">
+      <c r="K34" s="16"/>
+      <c r="L34" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="8" t="e">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="9" t="e">
+      <c r="I35" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J35" s="10" t="e">
+      <c r="J35" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="10">
+      <c r="K35" s="16"/>
+      <c r="L35" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="8" t="e">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I36" s="9" t="e">
+      <c r="I36" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J36" s="10" t="e">
+      <c r="J36" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K36" s="17"/>
-      <c r="L36" s="10">
+      <c r="K36" s="16"/>
+      <c r="L36" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="8" t="e">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I37" s="9" t="e">
+      <c r="I37" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J37" s="10" t="e">
+      <c r="J37" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K37" s="17"/>
-      <c r="L37" s="10">
+      <c r="K37" s="16"/>
+      <c r="L37" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="8" t="e">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="9" t="e">
+      <c r="I38" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J38" s="10" t="e">
+      <c r="J38" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="17"/>
-      <c r="L38" s="10">
+      <c r="K38" s="16"/>
+      <c r="L38" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="8" t="e">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I39" s="9" t="e">
+      <c r="I39" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J39" s="10" t="e">
+      <c r="J39" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K39" s="17"/>
-      <c r="L39" s="10">
+      <c r="K39" s="16"/>
+      <c r="L39" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="8" t="e">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="9" t="e">
+      <c r="I40" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J40" s="10" t="e">
+      <c r="J40" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K40" s="17"/>
-      <c r="L40" s="10">
+      <c r="K40" s="16"/>
+      <c r="L40" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="8" t="e">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="9" t="e">
+      <c r="I41" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J41" s="10" t="e">
+      <c r="J41" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K41" s="17"/>
-      <c r="L41" s="10">
+      <c r="K41" s="16"/>
+      <c r="L41" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="8" t="e">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="9" t="e">
+      <c r="I42" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J42" s="10" t="e">
+      <c r="J42" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K42" s="17"/>
-      <c r="L42" s="10">
+      <c r="K42" s="16"/>
+      <c r="L42" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="8" t="e">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I43" s="9" t="e">
+      <c r="I43" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J43" s="10" t="e">
+      <c r="J43" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K43" s="17"/>
-      <c r="L43" s="10">
+      <c r="K43" s="16"/>
+      <c r="L43" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="8" t="e">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I44" s="9" t="e">
+      <c r="I44" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J44" s="10" t="e">
+      <c r="J44" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K44" s="17"/>
-      <c r="L44" s="10">
+      <c r="K44" s="16"/>
+      <c r="L44" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="8" t="e">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I45" s="9" t="e">
+      <c r="I45" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J45" s="10" t="e">
+      <c r="J45" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K45" s="17"/>
-      <c r="L45" s="10">
+      <c r="K45" s="16"/>
+      <c r="L45" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="8" t="e">
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I46" s="9" t="e">
+      <c r="I46" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J46" s="10" t="e">
+      <c r="J46" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K46" s="17"/>
-      <c r="L46" s="10">
+      <c r="K46" s="16"/>
+      <c r="L46" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="8" t="e">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I47" s="9" t="e">
+      <c r="I47" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J47" s="10" t="e">
+      <c r="J47" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K47" s="17"/>
-      <c r="L47" s="10">
+      <c r="K47" s="16"/>
+      <c r="L47" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="8" t="e">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I48" s="9" t="e">
+      <c r="I48" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J48" s="10" t="e">
+      <c r="J48" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K48" s="17"/>
-      <c r="L48" s="10">
+      <c r="K48" s="16"/>
+      <c r="L48" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="8" t="e">
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="13" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I49" s="9" t="e">
+      <c r="I49" s="14" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J49" s="10" t="e">
+      <c r="J49" s="15" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K49" s="17"/>
-      <c r="L49" s="10">
+      <c r="K49" s="16"/>
+      <c r="L49" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="18"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="13" t="e">
+        <f t="shared" ref="H50:H100" si="10">AVERAGE(F50:G50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I50" s="14" t="e">
+        <f t="shared" ref="I50:I100" si="11">_xlfn.STDEV.S(F50:G50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J50" s="15" t="e">
+        <f t="shared" ref="J50:J100" si="12">100*I50/AVERAGE(F50:G50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K50" s="16"/>
+      <c r="L50" s="15">
+        <f t="shared" ref="L50:L100" si="13">E50*10^K50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="E51" s="11"/>
+      <c r="H51" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J51" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K51" s="16"/>
+      <c r="L51" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="E52" s="11"/>
+      <c r="H52" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J52" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K52" s="16"/>
+      <c r="L52" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="E53" s="11"/>
+      <c r="H53" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J53" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K53" s="16"/>
+      <c r="L53" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="E54" s="11"/>
+      <c r="H54" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J54" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K54" s="16"/>
+      <c r="L54" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="9"/>
+      <c r="E55" s="11"/>
+      <c r="H55" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I55" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J55" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K55" s="16"/>
+      <c r="L55" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="E56" s="11"/>
+      <c r="H56" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I56" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J56" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K56" s="16"/>
+      <c r="L56" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="E57" s="11"/>
+      <c r="H57" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I57" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J57" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K57" s="16"/>
+      <c r="L57" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="E58" s="11"/>
+      <c r="H58" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I58" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J58" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K58" s="16"/>
+      <c r="L58" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="E59" s="11"/>
+      <c r="H59" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I59" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J59" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K59" s="16"/>
+      <c r="L59" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="E60" s="11"/>
+      <c r="H60" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I60" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J60" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K60" s="16"/>
+      <c r="L60" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="E61" s="11"/>
+      <c r="H61" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I61" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J61" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K61" s="16"/>
+      <c r="L61" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="9"/>
+      <c r="E62" s="11"/>
+      <c r="H62" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I62" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J62" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K62" s="16"/>
+      <c r="L62" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="E63" s="11"/>
+      <c r="H63" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J63" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K63" s="16"/>
+      <c r="L63" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="9"/>
+      <c r="E64" s="11"/>
+      <c r="H64" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J64" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K64" s="16"/>
+      <c r="L64" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="9"/>
+      <c r="E65" s="11"/>
+      <c r="H65" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J65" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K65" s="16"/>
+      <c r="L65" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="B66" s="9"/>
+      <c r="E66" s="11"/>
+      <c r="H66" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J66" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K66" s="16"/>
+      <c r="L66" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="9"/>
+      <c r="E67" s="11"/>
+      <c r="H67" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J67" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K67" s="16"/>
+      <c r="L67" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="E68" s="11"/>
+      <c r="H68" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J68" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K68" s="16"/>
+      <c r="L68" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="E69" s="11"/>
+      <c r="H69" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J69" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K69" s="16"/>
+      <c r="L69" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="E70" s="11"/>
+      <c r="H70" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J70" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K70" s="16"/>
+      <c r="L70" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="9"/>
+      <c r="E71" s="11"/>
+      <c r="H71" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I71" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J71" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K71" s="16"/>
+      <c r="L71" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="E72" s="11"/>
+      <c r="H72" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I72" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J72" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K72" s="16"/>
+      <c r="L72" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="9"/>
+      <c r="E73" s="11"/>
+      <c r="H73" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I73" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J73" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K73" s="16"/>
+      <c r="L73" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9"/>
+      <c r="E74" s="11"/>
+      <c r="H74" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I74" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J74" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K74" s="16"/>
+      <c r="L74" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="B75" s="9"/>
+      <c r="E75" s="11"/>
+      <c r="H75" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I75" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J75" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K75" s="16"/>
+      <c r="L75" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="9"/>
+      <c r="E76" s="11"/>
+      <c r="H76" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I76" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J76" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K76" s="16"/>
+      <c r="L76" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="9"/>
+      <c r="E77" s="11"/>
+      <c r="H77" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I77" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J77" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K77" s="16"/>
+      <c r="L77" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+      <c r="E78" s="11"/>
+      <c r="H78" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I78" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J78" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K78" s="16"/>
+      <c r="L78" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
+      <c r="B79" s="9"/>
+      <c r="E79" s="11"/>
+      <c r="H79" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I79" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J79" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K79" s="16"/>
+      <c r="L79" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="8"/>
+      <c r="B80" s="9"/>
+      <c r="E80" s="11"/>
+      <c r="H80" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J80" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K80" s="16"/>
+      <c r="L80" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="8"/>
+      <c r="B81" s="9"/>
+      <c r="E81" s="11"/>
+      <c r="H81" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I81" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J81" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K81" s="16"/>
+      <c r="L81" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="8"/>
+      <c r="B82" s="9"/>
+      <c r="E82" s="11"/>
+      <c r="H82" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I82" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J82" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K82" s="16"/>
+      <c r="L82" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="8"/>
+      <c r="B83" s="9"/>
+      <c r="E83" s="11"/>
+      <c r="H83" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I83" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J83" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K83" s="16"/>
+      <c r="L83" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+      <c r="E84" s="11"/>
+      <c r="H84" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I84" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J84" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K84" s="16"/>
+      <c r="L84" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
+      <c r="B85" s="9"/>
+      <c r="E85" s="11"/>
+      <c r="H85" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I85" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J85" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K85" s="16"/>
+      <c r="L85" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+      <c r="E86" s="11"/>
+      <c r="H86" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I86" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J86" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K86" s="16"/>
+      <c r="L86" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
+      <c r="B87" s="9"/>
+      <c r="E87" s="11"/>
+      <c r="H87" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I87" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J87" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K87" s="16"/>
+      <c r="L87" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="E88" s="11"/>
+      <c r="H88" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I88" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J88" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K88" s="16"/>
+      <c r="L88" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="8"/>
+      <c r="B89" s="9"/>
+      <c r="E89" s="11"/>
+      <c r="H89" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I89" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J89" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K89" s="16"/>
+      <c r="L89" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="E90" s="11"/>
+      <c r="H90" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I90" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J90" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K90" s="16"/>
+      <c r="L90" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="8"/>
+      <c r="B91" s="9"/>
+      <c r="E91" s="11"/>
+      <c r="H91" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I91" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J91" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K91" s="16"/>
+      <c r="L91" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="E92" s="11"/>
+      <c r="H92" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I92" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J92" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K92" s="16"/>
+      <c r="L92" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="8"/>
+      <c r="B93" s="9"/>
+      <c r="E93" s="11"/>
+      <c r="H93" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I93" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J93" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K93" s="16"/>
+      <c r="L93" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="E94" s="11"/>
+      <c r="H94" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I94" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J94" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K94" s="16"/>
+      <c r="L94" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="8"/>
+      <c r="B95" s="9"/>
+      <c r="E95" s="11"/>
+      <c r="H95" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I95" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J95" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K95" s="16"/>
+      <c r="L95" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="E96" s="11"/>
+      <c r="H96" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I96" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J96" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K96" s="16"/>
+      <c r="L96" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
+      <c r="B97" s="9"/>
+      <c r="E97" s="11"/>
+      <c r="H97" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I97" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J97" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K97" s="16"/>
+      <c r="L97" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="E98" s="11"/>
+      <c r="H98" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I98" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J98" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K98" s="16"/>
+      <c r="L98" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="8"/>
+      <c r="B99" s="9"/>
+      <c r="E99" s="11"/>
+      <c r="H99" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I99" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J99" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K99" s="16"/>
+      <c r="L99" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
+      <c r="B100" s="9"/>
+      <c r="E100" s="11"/>
+      <c r="H100" s="13" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I100" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J100" s="15" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K100" s="16"/>
+      <c r="L100" s="15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J49">
+  <conditionalFormatting sqref="J2:J3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J100">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>15</formula>
     </cfRule>

</xml_diff>

<commit_message>
v1 multi fichiers fichier origine inclu erreur dans error tab
</commit_message>
<xml_diff>
--- a/multiplexSimoaGenerator/src/main/java/com/multiplexSimoaGenerator/neuro4plex_Model.xlsx
+++ b/multiplexSimoaGenerator/src/main/java/com/multiplexSimoaGenerator/neuro4plex_Model.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\git\mutiplexSimoaGenerator\multiplexSimoaGenerator\src\main\java\com\multiplexSimoaGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68CB453-68D4-459E-B87D-7C0DE8231F1C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB6B001-0A77-4C18-9E2B-5E6B026E8EF2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAB" sheetId="3" r:id="rId1"/>
     <sheet name="ERRORS" sheetId="9" r:id="rId2"/>
+    <sheet name="RAW DATA" sheetId="10" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ERRORS!$A$1:$AN$1</definedName>
@@ -1092,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3710,4 +3711,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732893A2-1A0A-4C81-B2EC-F2A4FD8BDD3D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>